<commit_message>
Adjust of some codes, inclusion of the quality codes and etc
</commit_message>
<xml_diff>
--- a/data/streamflow/estreams_streamflow_catalogue.xlsx
+++ b/data/streamflow/estreams_streamflow_catalogue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b65690e0ed38c20/PhD/Eawag/Papers/Paper1_Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E8BF892-272B-4BCB-BA57-5D31A4EE57F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C14E6D5-EA83-4050-B4A2-F22553A8D8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{440C78F0-496D-5848-B483-D1372D576F79}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="471">
   <si>
     <t>provider_id</t>
   </si>
@@ -424,6 +424,9 @@
     <t>Bayerisches Landesamt fur Umwelt (GKD Bayern)</t>
   </si>
   <si>
+    <t>Redristribution allowed</t>
+  </si>
+  <si>
     <t>https://www.gkd.bayern.de/en/</t>
   </si>
   <si>
@@ -880,16 +883,22 @@
     <t>OPW. Office of Public Works, Ireland. https://waterlevel.ie/hydro-data (last access: 27 Jun 2023).</t>
   </si>
   <si>
-    <t>IS_GRDC</t>
-  </si>
-  <si>
-    <t>ISGR</t>
+    <t>IS_LAMAHICE</t>
+  </si>
+  <si>
+    <t>IS</t>
   </si>
   <si>
     <t>ICELAND</t>
   </si>
   <si>
-    <t>IS</t>
+    <t>LArge-SaMple DAta for Hydrology and Environmental Sciences for Iceland (LamaH-Ice)</t>
+  </si>
+  <si>
+    <t>http://www.hydroshare.org/resource/86117a5f36cc4b7c90a5d54e18161c91</t>
+  </si>
+  <si>
+    <t>Helgason, H. B. and Nijssen, B.: LamaH-Ice: LArge-SaMple Data for Hydrology and Environmental Sciences for Iceland [data set], http://www.hydroshare.org/resource/86117a5f36cc4b7c90a5d54e18161c91, 2023 (last access: 29 Apr 2024).</t>
   </si>
   <si>
     <t>IT_ABR_CONTACTFORM</t>
@@ -1348,25 +1357,19 @@
     <t>RO</t>
   </si>
   <si>
-    <t>RS_RHMS</t>
+    <t>RS_GDRC</t>
+  </si>
+  <si>
+    <t>RSGR</t>
+  </si>
+  <si>
+    <t>SERBIA</t>
   </si>
   <si>
     <t>RS</t>
   </si>
   <si>
-    <t>SERBIA</t>
-  </si>
-  <si>
-    <t>Republic Hydrometeorological Service of Serbia (RHMS)</t>
-  </si>
-  <si>
-    <t>https://www.hidmet.gov.rs</t>
-  </si>
-  <si>
-    <t>https://www.hidmet.gov.rs/latin/hidrologija/povrsinske_godisnjaci.php</t>
-  </si>
-  <si>
-    <t>RHSS. Republic Hydrometeorological Service of Serbia. https://www.hidmet.gov.rs/latin/hidrologija/povrsinske_godisnjaci.php (last access: 23 Jun 2023).</t>
+    <t>GRDC. Global Runoff Data Center: River discharge data. Federal Institute of Hydrology, 56068 Koblenz, Germany. https://www.bafg.de/GRDC (last access: 29 Apr 2024).</t>
   </si>
   <si>
     <t>RU_GRDC</t>
@@ -1634,12 +1637,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1663,15 +1665,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1987,8 +1986,8 @@
   <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E56" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K64" sqref="K64"/>
+      <pane xSplit="1" topLeftCell="C23" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2628,7 +2627,7 @@
         <v>108</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>21</v>
@@ -2637,25 +2636,25 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>_xlfn.CONCAT(LEFT(A16,2), RIGHT(A16,2))</f>
@@ -2668,7 +2667,7 @@
         <v>87</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>20</v>
@@ -2680,25 +2679,25 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>_xlfn.CONCAT(LEFT(A17,2), RIGHT(A17,2))</f>
@@ -2711,7 +2710,7 @@
         <v>87</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>89</v>
@@ -2723,25 +2722,25 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>_xlfn.CONCAT(LEFT(A18,2), RIGHT(A18,2))</f>
@@ -2754,7 +2753,7 @@
         <v>87</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>89</v>
@@ -2766,25 +2765,25 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>_xlfn.CONCAT(LEFT(A19,2), RIGHT(A19,2))</f>
@@ -2797,10 +2796,10 @@
         <v>87</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>21</v>
@@ -2809,25 +2808,25 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="P19" s="4"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>_xlfn.CONCAT(LEFT(A20,2), RIGHT(A20,2))</f>
@@ -2840,7 +2839,7 @@
         <v>87</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>102</v>
@@ -2852,25 +2851,25 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>_xlfn.CONCAT(LEFT(A21,2), RIGHT(A21,2))</f>
@@ -2883,7 +2882,7 @@
         <v>87</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>102</v>
@@ -2895,25 +2894,25 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P21" s="4"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B22" s="4" t="str">
         <f t="shared" ref="B22:B24" si="0">_xlfn.CONCAT(LEFT(A22,2), RIGHT(A22,2))</f>
@@ -2926,37 +2925,37 @@
         <v>87</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L22" t="s">
         <v>20</v>
       </c>
       <c r="M22" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2969,37 +2968,37 @@
         <v>87</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3012,52 +3011,52 @@
         <v>87</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
       <c r="K24" s="15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>21</v>
@@ -3066,36 +3065,36 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L25" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="M25" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="M25" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="N25" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>55</v>
@@ -3128,19 +3127,19 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>179</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>20</v>
@@ -3152,42 +3151,42 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>21</v>
@@ -3196,39 +3195,39 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="E29" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>20</v>
@@ -3240,37 +3239,37 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O29" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P29" s="4"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="E30" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>38</v>
@@ -3282,36 +3281,36 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>55</v>
@@ -3344,19 +3343,19 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>215</v>
-      </c>
       <c r="E32" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>38</v>
@@ -3368,37 +3367,37 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O32" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>20</v>
@@ -3410,37 +3409,37 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O33" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P33" s="4"/>
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>229</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>20</v>
@@ -3452,76 +3451,76 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L34" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="M34" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="N34" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O34" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="P34" s="4"/>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="O35" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="P35" s="4"/>
     </row>
     <row r="36" spans="1:16">
       <c r="A36" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>55</v>
@@ -3554,22 +3553,22 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>21</v>
@@ -3578,40 +3577,40 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="O37" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="P37" s="4"/>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>21</v>
@@ -3620,40 +3619,40 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="P38" s="4"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="E39" s="6" t="s">
-        <v>55</v>
+        <v>265</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>21</v>
@@ -3662,79 +3661,79 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="5" t="s">
-        <v>56</v>
+        <v>266</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>57</v>
+        <v>266</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>56</v>
+        <v>266</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>56</v>
+        <v>266</v>
       </c>
       <c r="O39" s="12" t="s">
-        <v>58</v>
+        <v>267</v>
       </c>
       <c r="P39" s="4"/>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="O40" s="12" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P40" s="4"/>
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="6" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>20</v>
@@ -3746,34 +3745,34 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="P41" s="4"/>
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="6" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>55</v>
@@ -3806,19 +3805,19 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="6" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>20</v>
@@ -3830,81 +3829,81 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="15" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="N43" s="17" t="s">
-        <v>285</v>
+        <v>288</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>288</v>
       </c>
       <c r="O43" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="P43" s="16" t="s">
-        <v>287</v>
+        <v>289</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="6" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="5" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="N44" s="19" t="s">
-        <v>292</v>
+        <v>295</v>
+      </c>
+      <c r="N44" s="17" t="s">
+        <v>295</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="P44" s="4"/>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>20</v>
@@ -3916,82 +3915,82 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="5" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="O45" s="12" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="P45" s="4"/>
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="5" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="O46" s="12" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="P46" s="4"/>
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="6" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>21</v>
@@ -4000,37 +3999,37 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O47" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="P47" s="4"/>
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>20</v>
@@ -4042,37 +4041,37 @@
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O48" s="12" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="P48" s="4"/>
     </row>
     <row r="49" spans="1:16">
       <c r="A49" s="6" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>20</v>
@@ -4084,40 +4083,40 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="5" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="O49" s="12" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="P49" s="4"/>
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="6" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>21</v>
@@ -4126,37 +4125,37 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="N50" s="18" t="s">
-        <v>333</v>
+        <v>335</v>
+      </c>
+      <c r="N50" s="16" t="s">
+        <v>336</v>
       </c>
       <c r="O50" s="12" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="P50" s="4"/>
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="6" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>20</v>
@@ -4168,37 +4167,37 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="5" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="L51" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="O51" s="12" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="P51" s="4"/>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="6" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>20</v>
@@ -4210,76 +4209,76 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="L52" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="O52" s="12" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="P52" s="4"/>
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="6" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="L53" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="O53" s="12" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="P53" s="4"/>
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="6" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>55</v>
@@ -4312,58 +4311,58 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55" s="6" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="5" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="O55" s="4" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="P55" s="4"/>
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="6" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>55</v>
@@ -4396,16 +4395,16 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="6" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>55</v>
@@ -4438,16 +4437,16 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="6" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>55</v>
@@ -4480,19 +4479,19 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="6" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>38</v>
@@ -4504,42 +4503,42 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O59" s="12" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="P59" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="6" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>21</v>
@@ -4548,40 +4547,40 @@
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="5" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="N60" s="5" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="O60" s="12" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="P60" s="4"/>
     </row>
     <row r="61" spans="1:16">
       <c r="A61" s="6" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>21</v>
@@ -4590,37 +4589,37 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="5" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="O61" s="12" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="P61" s="4"/>
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="6" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>20</v>
@@ -4632,37 +4631,37 @@
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="5" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="O62" s="12" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="P62" s="4"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="6" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>20</v>
@@ -4674,36 +4673,36 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="15" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="L63" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="O63" s="12" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="P63" s="4" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="6" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>55</v>
@@ -4736,22 +4735,22 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" s="6" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>420</v>
+        <v>55</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>21</v>
@@ -4760,34 +4759,34 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="L65" s="7" t="s">
-        <v>183</v>
+        <v>56</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>422</v>
+        <v>56</v>
       </c>
       <c r="N65" s="5" t="s">
-        <v>422</v>
+        <v>56</v>
       </c>
       <c r="O65" s="12" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="P65" s="4"/>
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="6" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>55</v>
@@ -4820,22 +4819,22 @@
     </row>
     <row r="67" spans="1:16">
       <c r="A67" s="6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C67" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>429</v>
-      </c>
       <c r="E67" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>21</v>
@@ -4844,37 +4843,37 @@
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="5" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="N67" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O67" s="12" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P67" s="4"/>
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C68" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="D68" s="4" t="s">
-        <v>437</v>
-      </c>
       <c r="E68" s="6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>20</v>
@@ -4886,34 +4885,34 @@
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="L68" s="5" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="N68" s="5" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="O68" s="12" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="P68" s="4"/>
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="6" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>55</v>
@@ -4946,16 +4945,16 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" s="6" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>55</v>
@@ -4988,16 +4987,16 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="6" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>55</v>
@@ -5047,214 +5046,209 @@
     <hyperlink ref="M2" r:id="rId12" xr:uid="{2D2F929C-7D44-4186-8ADF-369BF910DFF3}"/>
     <hyperlink ref="M67" r:id="rId13" location="param=waterdischargeDaily,stations=core" xr:uid="{B310E1C2-0A0C-47DC-9853-C2F9771FAFE1}"/>
     <hyperlink ref="N67" r:id="rId14" location="param=waterdischargeDaily,stations=core" xr:uid="{51FA1969-D853-47FD-98AA-B8E89B09CEA4}"/>
-    <hyperlink ref="M39" r:id="rId15" xr:uid="{08F4D0FF-B05E-4C92-B91A-9B0DC534023E}"/>
-    <hyperlink ref="N39" r:id="rId16" xr:uid="{C7A9AACB-FA33-4C8D-A6A1-44CCE005EAB9}"/>
-    <hyperlink ref="N38" r:id="rId17" xr:uid="{36425243-7AC7-4AF2-9C5E-4565F4976C81}"/>
-    <hyperlink ref="M34" r:id="rId18" xr:uid="{DBC2D6E2-BCC2-4A50-AB7D-56020DB587FB}"/>
-    <hyperlink ref="N34" r:id="rId19" xr:uid="{2D27D948-C2E5-4F8F-B314-E0ED6384AC1F}"/>
-    <hyperlink ref="M36" r:id="rId20" xr:uid="{A07E8140-BA13-4365-A072-4B3986562265}"/>
-    <hyperlink ref="N36" r:id="rId21" xr:uid="{0971B232-3558-426C-9785-F42E3B282419}"/>
-    <hyperlink ref="M11" r:id="rId22" xr:uid="{279476CE-E1C0-48C4-818D-89FB1F97F961}"/>
-    <hyperlink ref="N11" r:id="rId23" xr:uid="{C2B01C9A-4FD2-4B15-97DE-BA135F48781E}"/>
-    <hyperlink ref="M10" r:id="rId24" xr:uid="{5B7AD2FF-5DC0-4759-B8EB-6920748A04B0}"/>
-    <hyperlink ref="N10" r:id="rId25" xr:uid="{097020E7-7110-420E-8F4F-22705FF1C983}"/>
-    <hyperlink ref="M62" r:id="rId26" xr:uid="{55DBDEEF-2AAE-4826-A696-5AF28C579F2C}"/>
-    <hyperlink ref="N62" r:id="rId27" xr:uid="{32491A74-5E35-40A2-B784-3C602FE3803E}"/>
-    <hyperlink ref="M56" r:id="rId28" xr:uid="{3326CBF8-3EB1-43A4-99CF-B30D34390DF0}"/>
-    <hyperlink ref="N56" r:id="rId29" xr:uid="{F04B0833-9438-4AA9-AD19-3E9519B662DF}"/>
-    <hyperlink ref="M26" r:id="rId30" xr:uid="{5FC295D2-0A87-43CF-B54E-E04FDEF3C086}"/>
-    <hyperlink ref="N26" r:id="rId31" xr:uid="{C69B99EC-6AAD-4348-9878-CF4948DF912F}"/>
-    <hyperlink ref="M54" r:id="rId32" xr:uid="{DA4E132F-427D-48CE-8AE5-D57D5345B0DE}"/>
-    <hyperlink ref="N54" r:id="rId33" xr:uid="{16EC9894-554A-476B-9997-8B010A26937D}"/>
-    <hyperlink ref="M65" r:id="rId34" xr:uid="{A4D679C4-63C9-4ADC-A124-A2C19ABC7E84}"/>
-    <hyperlink ref="N65" r:id="rId35" xr:uid="{25E1B893-6062-4491-8C1F-7BA009350AD1}"/>
-    <hyperlink ref="M28" r:id="rId36" xr:uid="{F7E5D8C3-2441-43E4-9EED-A75357EFBB21}"/>
-    <hyperlink ref="N17" r:id="rId37" xr:uid="{F05D6F16-F886-423C-ABF2-038F3B1CDEF4}"/>
-    <hyperlink ref="M17" r:id="rId38" xr:uid="{19BB88FF-CE20-4D1B-B657-42E6BD33C36F}"/>
-    <hyperlink ref="M15" r:id="rId39" xr:uid="{B0E0B30B-E083-40BC-8AA7-3338372CC3CC}"/>
-    <hyperlink ref="M13" r:id="rId40" xr:uid="{3DC141FD-85DD-4383-BEDB-EC3FFE27AAE3}"/>
-    <hyperlink ref="M12" r:id="rId41" xr:uid="{A1EEA0E6-B203-496D-BE05-7E8400174743}"/>
-    <hyperlink ref="M16" r:id="rId42" location="/overview/Wasserstand?mode=table&amp;filter=%7B%7D" xr:uid="{431514AB-B3FA-4FA0-9FAD-440C154FA405}"/>
-    <hyperlink ref="M18" r:id="rId43" xr:uid="{7D99DF82-54F7-43C9-BDF5-7393A84867EC}"/>
-    <hyperlink ref="M20" r:id="rId44" display="https://www.umwelt.sachsen.de/umwelt/infosysteme/ida/processingChain?conditionValuesSetHash=0A8BBED&amp;selector=ROOT.Thema%20Wasser.Oberirdische%20Gew%C3%A4sser.Pegel.Wasserstand%20und%20Durchfluss.OWMN%3Aowmn_menge_tagesmittelwerte_v2.sel&amp;sourceOrderAsc=false&amp;columns=9dfa2224-c924-4328-9805-1d34cd748026&amp;offset=0&amp;limit=2147483647&amp;executionConfirmed=false" xr:uid="{C35973C5-6A64-44EE-A724-C69D5BE3F7E6}"/>
-    <hyperlink ref="M21" r:id="rId45" xr:uid="{B3C90335-1BE9-48EA-B27B-E90DCED2E7E3}"/>
-    <hyperlink ref="M19" r:id="rId46" xr:uid="{39535A38-FA1B-4791-9CCF-AC09009FE4BD}"/>
-    <hyperlink ref="L20" r:id="rId47" xr:uid="{207D6C47-461A-4FB0-91AA-E9190D4AD299}"/>
-    <hyperlink ref="L14" r:id="rId48" xr:uid="{883314B1-D5D9-4628-87D5-DDE64206486E}"/>
-    <hyperlink ref="M41" r:id="rId49" xr:uid="{43926695-05CD-4BBA-8DFE-708730AA56A4}"/>
-    <hyperlink ref="M45" r:id="rId50" xr:uid="{7532A1D1-B3CC-4D73-9197-D5031B40BFAF}"/>
-    <hyperlink ref="M48" r:id="rId51" xr:uid="{47C217E4-5192-4BC5-B8DB-1689774C34DE}"/>
-    <hyperlink ref="M49" r:id="rId52" xr:uid="{0DD9DAEA-2C6C-40E8-A164-8A68BA4C893A}"/>
-    <hyperlink ref="M50" r:id="rId53" xr:uid="{D0121DD0-D1A3-4DEE-B23A-F2D5D3ABBD96}"/>
-    <hyperlink ref="M51" r:id="rId54" xr:uid="{E41A3D15-0340-41E2-98A7-F8398F4A755D}"/>
-    <hyperlink ref="N52" r:id="rId55" xr:uid="{4DAC29CC-FA65-4308-9D93-678CFFA252D6}"/>
-    <hyperlink ref="N53" r:id="rId56" xr:uid="{C40CB76B-AB6D-4BA4-8907-DED5472C6E97}"/>
-    <hyperlink ref="M3" r:id="rId57" xr:uid="{33FB1494-C397-4B17-91BC-5FE74371668D}"/>
-    <hyperlink ref="M4" r:id="rId58" xr:uid="{B8E3B2CA-F963-4B0E-8C02-4C03E1227DF4}"/>
-    <hyperlink ref="N4" r:id="rId59" xr:uid="{729A8956-37E0-4833-8991-3B8568AAFDC5}"/>
-    <hyperlink ref="M5" r:id="rId60" xr:uid="{D3531896-F25D-4B11-8143-46178B99F492}"/>
-    <hyperlink ref="M25" r:id="rId61" xr:uid="{C52B4BD9-0874-4857-AC72-F04C4D64C703}"/>
-    <hyperlink ref="M32" r:id="rId62" xr:uid="{6E3D0688-22E8-4E62-B6CA-7826AC97D1BD}"/>
-    <hyperlink ref="M33" r:id="rId63" xr:uid="{B0E296EC-DA7A-4CDB-B302-AB0BCA9A449C}"/>
-    <hyperlink ref="M37" r:id="rId64" location="Flow" xr:uid="{CDF25C43-EC31-4721-9269-ADC87A23284B}"/>
-    <hyperlink ref="M38" r:id="rId65" xr:uid="{74B57653-6E77-49EA-ACF6-F96EBEF7ABD0}"/>
-    <hyperlink ref="N37" r:id="rId66" location="Flow" xr:uid="{3A19F3BE-B518-49A6-B35C-315D0EA8F950}"/>
-    <hyperlink ref="M60" r:id="rId67" location="/publiek/waterafvoer" xr:uid="{96586330-2B0F-4F2C-8680-F6817AEB8F04}"/>
-    <hyperlink ref="M61" r:id="rId68" xr:uid="{7CC951DB-46BB-4141-91A9-CAD87A9630C2}"/>
-    <hyperlink ref="N63" r:id="rId69" xr:uid="{789C1C9F-19EE-4C2D-8BD8-94FE0B3FC6AE}"/>
-    <hyperlink ref="N68" r:id="rId70" xr:uid="{A13F99C2-CBCA-4A9C-98C1-BFCC028A369E}"/>
-    <hyperlink ref="L2" r:id="rId71" xr:uid="{0299DE14-E216-4750-86E9-8D8EB4F2F60F}"/>
-    <hyperlink ref="L4" r:id="rId72" xr:uid="{DF7D6F98-A06C-4878-8DB9-D216C854E14D}"/>
-    <hyperlink ref="L5" r:id="rId73" xr:uid="{6881C1FC-83D3-4B48-A703-2E808EF26433}"/>
-    <hyperlink ref="L6" r:id="rId74" xr:uid="{EE8683AF-647E-44D0-9AAF-DE6C59A8E670}"/>
-    <hyperlink ref="L7" r:id="rId75" xr:uid="{DA89D6B4-E546-4384-833D-5B981EB9F619}"/>
-    <hyperlink ref="L9" r:id="rId76" xr:uid="{9DBBDB5C-6C84-4AB3-A69C-456D02F16E75}"/>
-    <hyperlink ref="L11" r:id="rId77" xr:uid="{D6A5B413-7EA0-43FE-AB42-21F8D0E984F9}"/>
-    <hyperlink ref="L26" r:id="rId78" xr:uid="{FEC4CB21-36E5-4529-9BD1-0965488594A6}"/>
-    <hyperlink ref="L31" r:id="rId79" xr:uid="{F8CEB9F3-7B0C-4D96-A220-52A24EAC71E7}"/>
-    <hyperlink ref="L36" r:id="rId80" xr:uid="{EA1D39A9-DDA4-45AC-8128-015822DB9A5D}"/>
-    <hyperlink ref="L39" r:id="rId81" xr:uid="{2D72B67F-327C-44CF-88C0-27D00065D352}"/>
-    <hyperlink ref="L42" r:id="rId82" xr:uid="{6F22F521-9893-41B8-A862-C1942E31D4BF}"/>
-    <hyperlink ref="L54" r:id="rId83" xr:uid="{096C2498-87C2-4EF8-BA1F-5292F90C701F}"/>
-    <hyperlink ref="L56" r:id="rId84" xr:uid="{FCCB7294-9C23-47BB-B1C6-60A7018BA619}"/>
-    <hyperlink ref="L57" r:id="rId85" xr:uid="{05116FA7-B29F-4F36-AF29-282D72A106D9}"/>
-    <hyperlink ref="L58" r:id="rId86" xr:uid="{6C2CBE78-01AB-4051-8C7B-42327679A546}"/>
-    <hyperlink ref="L64" r:id="rId87" xr:uid="{923E7558-C9F5-45F4-83BD-D269E0DB6478}"/>
-    <hyperlink ref="L66" r:id="rId88" xr:uid="{F538C2FD-1BF4-46EA-9EE2-7BD3FC3454AF}"/>
-    <hyperlink ref="L69" r:id="rId89" xr:uid="{89748D0F-FE77-4F73-88FF-D48215C8E0C4}"/>
-    <hyperlink ref="L70" r:id="rId90" xr:uid="{D040ECFD-5D11-440E-903F-88818593C862}"/>
-    <hyperlink ref="L71" r:id="rId91" xr:uid="{D7BDD944-60B6-4AF0-853D-1A3F20EF5B74}"/>
-    <hyperlink ref="L8" r:id="rId92" xr:uid="{D00FA835-7423-4F1B-A2F7-7CA692EB4D08}"/>
-    <hyperlink ref="L10" r:id="rId93" xr:uid="{0950615F-A860-49D2-8DC3-F1A766019300}"/>
-    <hyperlink ref="L25" r:id="rId94" xr:uid="{6F5B7FA1-7FF8-45A0-AD6F-DAB544653875}"/>
-    <hyperlink ref="L28" r:id="rId95" xr:uid="{E23A4653-97A1-4A9C-9A5E-86DB637385CD}"/>
-    <hyperlink ref="L30" r:id="rId96" xr:uid="{B4AD2D64-E0A7-42D7-8193-9DFA2C7DC3E3}"/>
-    <hyperlink ref="L32" r:id="rId97" xr:uid="{908964D2-BFBF-4D62-8C00-9DB0F3CF8F4C}"/>
-    <hyperlink ref="L34" r:id="rId98" xr:uid="{5EAC2889-2641-4CD3-AF8D-76999ADB2175}"/>
-    <hyperlink ref="L37" r:id="rId99" location="Disclaimer" xr:uid="{3D3FE31F-229F-4DF0-B134-74A89311E685}"/>
-    <hyperlink ref="L38" r:id="rId100" location="license" xr:uid="{B99B8BD6-D4A5-453B-AE98-CC9D29CF5153}"/>
-    <hyperlink ref="L60" r:id="rId101" location="/copyright" xr:uid="{FC405A94-92ED-4C9A-B03B-2E789AC1840B}"/>
-    <hyperlink ref="L61" r:id="rId102" xr:uid="{4679CB8D-3930-4582-8DC6-6CCCD9244845}"/>
-    <hyperlink ref="L62" r:id="rId103" xr:uid="{FEB0A51B-B691-42DE-BB37-0046CEF421D3}"/>
-    <hyperlink ref="L67" r:id="rId104" xr:uid="{4052B3D9-0526-4DBE-864A-2CC2235E7A37}"/>
-    <hyperlink ref="L68" r:id="rId105" xr:uid="{CCC7D3D2-0EC0-4146-A122-99610EFB2686}"/>
-    <hyperlink ref="L15" r:id="rId106" xr:uid="{56B414F3-175F-401F-8F3A-B8C78A7999CD}"/>
-    <hyperlink ref="L13" r:id="rId107" xr:uid="{A4EAB253-FEFD-4D34-80C7-7BA329647C14}"/>
-    <hyperlink ref="L12" r:id="rId108" xr:uid="{96A4267D-73B0-4C6F-9E07-E63600BC735E}"/>
-    <hyperlink ref="L17" r:id="rId109" xr:uid="{0197946F-7B35-4321-9287-CDA7E7C977D4}"/>
-    <hyperlink ref="L18" r:id="rId110" xr:uid="{055CF3B6-9FBF-4B8C-8FD8-0AAB65FAA1E5}"/>
-    <hyperlink ref="L19" r:id="rId111" xr:uid="{3A2597C8-4F13-4689-9AFE-21B00D45BEED}"/>
-    <hyperlink ref="L21" r:id="rId112" xr:uid="{36911D06-4E86-4336-AB05-DEEFC03993C4}"/>
-    <hyperlink ref="M47" r:id="rId113" xr:uid="{EEE7B747-EA92-4E2F-8DD2-42A7E93FC151}"/>
-    <hyperlink ref="L47" r:id="rId114" xr:uid="{7CEF2492-538E-4BAD-9D26-C242373BBC4E}"/>
-    <hyperlink ref="L50" r:id="rId115" xr:uid="{DF4077F2-C770-40DD-A27F-83A17C16C2E5}"/>
-    <hyperlink ref="L48" r:id="rId116" xr:uid="{5914BA4C-2BA2-43E3-89D7-0D6B9190240E}"/>
-    <hyperlink ref="N49" r:id="rId117" xr:uid="{A817B0D0-793B-4CEB-A87B-CC6EB2B9F74F}"/>
-    <hyperlink ref="M52" r:id="rId118" xr:uid="{15DC8865-310D-4087-8466-6245886B5D29}"/>
-    <hyperlink ref="M40" r:id="rId119" xr:uid="{06D3FF73-6B12-4BBB-A197-CA12AD356B9D}"/>
-    <hyperlink ref="L35" r:id="rId120" xr:uid="{3D0FC602-9EAD-4C95-ACD5-A517F3CA367E}"/>
-    <hyperlink ref="M35" r:id="rId121" xr:uid="{5225E5E6-68CA-45D3-957A-E0E37EA3F330}"/>
-    <hyperlink ref="N35" r:id="rId122" xr:uid="{1B63C25C-317F-43E7-B1F7-5EC348C8D37F}"/>
-    <hyperlink ref="N12" r:id="rId123" xr:uid="{5191E8D6-EFCE-47F2-BFDD-65E782D29C97}"/>
-    <hyperlink ref="N13" r:id="rId124" xr:uid="{AC024018-7240-4497-9263-E5140DE193E2}"/>
-    <hyperlink ref="N14" r:id="rId125" xr:uid="{8A87FECF-B3BD-4862-B096-08E217FACC71}"/>
-    <hyperlink ref="N15" r:id="rId126" xr:uid="{B76E7E82-13F4-49FF-B9D8-936CACFEE75B}"/>
-    <hyperlink ref="N16" r:id="rId127" location="/overview/Wasserstand?mode=table&amp;filter=%7B%7D" xr:uid="{A702C0F3-C827-4E97-926E-3859C4A9F3A6}"/>
-    <hyperlink ref="N18" r:id="rId128" xr:uid="{1BDC5B18-0D62-4B9D-B3FC-EF429CD15631}"/>
-    <hyperlink ref="N19" r:id="rId129" xr:uid="{432A0A37-FCCE-437D-8B15-29AAEBAFAFEF}"/>
-    <hyperlink ref="N20" r:id="rId130" display="https://www.umwelt.sachsen.de/umwelt/infosysteme/ida/processingChain?conditionValuesSetHash=0A8BBED&amp;selector=ROOT.Thema%20Wasser.Oberirdische%20Gew%C3%A4sser.Pegel.Wasserstand%20und%20Durchfluss.OWMN%3Aowmn_menge_tagesmittelwerte_v2.sel&amp;sourceOrderAsc=false&amp;columns=9dfa2224-c924-4328-9805-1d34cd748026&amp;offset=0&amp;limit=2147483647&amp;executionConfirmed=false" xr:uid="{44371C46-89E1-42BB-8255-2F19865CAC42}"/>
-    <hyperlink ref="N21" r:id="rId131" xr:uid="{4E9346F0-3C12-486C-80E9-1D27EF91D279}"/>
-    <hyperlink ref="N28" r:id="rId132" xr:uid="{0548E784-EC86-422C-AEFF-0EB8A5B0B2D6}"/>
-    <hyperlink ref="M46" r:id="rId133" xr:uid="{EA54538E-62F8-4C22-8A62-E9926A6A5737}"/>
-    <hyperlink ref="K2" r:id="rId134" xr:uid="{39BD2D35-9444-4862-A80F-55A1E85CDBC1}"/>
-    <hyperlink ref="K3" r:id="rId135" xr:uid="{7CD1346D-FDE6-4779-937A-01DE1647C6BE}"/>
-    <hyperlink ref="K4" r:id="rId136" xr:uid="{664B96AA-17CD-4E97-8794-2B528D15B646}"/>
-    <hyperlink ref="K5" r:id="rId137" xr:uid="{95D42C21-00AD-4526-AF1D-1245D8BBDBAC}"/>
-    <hyperlink ref="K6" r:id="rId138" xr:uid="{74B0C055-27A6-4831-BF2E-BEB7443EC0BF}"/>
-    <hyperlink ref="K7" r:id="rId139" xr:uid="{53240E1F-B2EA-4CBB-BC4D-11DF789DE658}"/>
-    <hyperlink ref="K8" r:id="rId140" xr:uid="{A4D39D4C-3051-4EA7-8C35-A9F991BFE999}"/>
-    <hyperlink ref="K9" r:id="rId141" xr:uid="{7BD9B41B-78AE-4FFA-820D-B582535F5787}"/>
-    <hyperlink ref="K11" r:id="rId142" xr:uid="{A2FF850A-9C56-426B-A8D3-7699203241CA}"/>
-    <hyperlink ref="K26" r:id="rId143" xr:uid="{A9A6F852-880A-46EE-A4C6-77C5718A3201}"/>
-    <hyperlink ref="K31" r:id="rId144" xr:uid="{3E3F1C4F-BC6F-40BB-906B-FC038E31F7FA}"/>
-    <hyperlink ref="K36" r:id="rId145" xr:uid="{205D0983-3D75-4845-A2B7-F2FE9CDE7471}"/>
-    <hyperlink ref="K39" r:id="rId146" xr:uid="{79A36E04-ECCA-4B91-9919-B73476E5FDE4}"/>
-    <hyperlink ref="K42" r:id="rId147" xr:uid="{5981BD4E-3A64-4044-8F00-D6CA30DFA79D}"/>
-    <hyperlink ref="K54" r:id="rId148" xr:uid="{7FB92A2C-7602-4910-82F1-6CEDDF5D9B9A}"/>
-    <hyperlink ref="K56" r:id="rId149" xr:uid="{67C930FE-1C69-449C-B47B-4A7A250402E9}"/>
-    <hyperlink ref="K57" r:id="rId150" xr:uid="{84C56357-09DE-4C90-85DB-1792BB5FD67E}"/>
-    <hyperlink ref="K58" r:id="rId151" xr:uid="{5F7107D3-8EFA-4786-84E2-A6989793C4C1}"/>
-    <hyperlink ref="K64" r:id="rId152" xr:uid="{BB77463F-FCF5-4AB6-87DD-898851A69AAF}"/>
-    <hyperlink ref="K66" r:id="rId153" xr:uid="{B0FC0A8B-D1B5-43EB-8ACC-94F2484F2473}"/>
-    <hyperlink ref="K69" r:id="rId154" xr:uid="{87F3D8E6-B39E-422F-9126-E039037C3E60}"/>
-    <hyperlink ref="K70" r:id="rId155" xr:uid="{01C03372-5C1F-4B2B-B3A5-EBDAC3883D12}"/>
-    <hyperlink ref="K71" r:id="rId156" xr:uid="{37BC70ED-F49B-4D64-A2FC-DCFD47E4FED3}"/>
-    <hyperlink ref="K10" r:id="rId157" xr:uid="{C7CF1733-E812-4526-876F-58DD8A4833F5}"/>
-    <hyperlink ref="K12" r:id="rId158" xr:uid="{A78CA3AE-B607-4503-AE9C-F1BAB092660D}"/>
-    <hyperlink ref="K13" r:id="rId159" xr:uid="{90B567F9-2099-45DB-BC2A-F72365264C51}"/>
-    <hyperlink ref="K14" r:id="rId160" xr:uid="{4DABE13E-10F9-472D-AFC4-2194D25E99D4}"/>
-    <hyperlink ref="K15" r:id="rId161" xr:uid="{63F30CC4-6855-4998-8F05-CF67C966A2C0}"/>
-    <hyperlink ref="K16" r:id="rId162" xr:uid="{18AA6A95-4D23-4770-A296-75B7DCB97DD7}"/>
-    <hyperlink ref="K17" r:id="rId163" xr:uid="{C1F270AF-7F6D-4162-80BC-558BF58E1E7C}"/>
-    <hyperlink ref="K18" r:id="rId164" xr:uid="{7E85EBA1-47D1-4E78-9C9F-CBD8CFB9A33A}"/>
-    <hyperlink ref="K19" r:id="rId165" xr:uid="{538A5124-FD86-47B8-9C9C-74CD88DACC39}"/>
-    <hyperlink ref="K20" r:id="rId166" xr:uid="{2EAE1522-545A-4EDF-8035-59C73436A4E2}"/>
-    <hyperlink ref="K21" r:id="rId167" xr:uid="{02F0BCE1-47EA-4B5C-804D-63003D4E1256}"/>
-    <hyperlink ref="K25" r:id="rId168" xr:uid="{14C3752A-1073-4D2C-A4B1-6241C66A0956}"/>
-    <hyperlink ref="K27" r:id="rId169" xr:uid="{0A765B89-5D1E-4011-A3BE-F4A4A4943B63}"/>
-    <hyperlink ref="N27" r:id="rId170" xr:uid="{9BAF5DDB-652F-4D4E-903E-C9CFA2E50E7A}"/>
-    <hyperlink ref="K28" r:id="rId171" xr:uid="{848721C6-ABF0-45B7-B5C2-EB7EFBE5073B}"/>
-    <hyperlink ref="K29" r:id="rId172" xr:uid="{E36B8C29-A364-4F36-8A5A-52E09808BEED}"/>
-    <hyperlink ref="K30" r:id="rId173" xr:uid="{E8ED1CD5-2249-4B8B-9940-6E1A699441C1}"/>
-    <hyperlink ref="K32" r:id="rId174" xr:uid="{F057875F-AA86-468C-97C4-935E7ADDCDF1}"/>
-    <hyperlink ref="K33" r:id="rId175" xr:uid="{FDD7E05C-4786-4A71-B881-CEC77A8E45BE}"/>
-    <hyperlink ref="K34" r:id="rId176" xr:uid="{96BD0EB1-795E-42C6-BBB6-EF0E987EAD0F}"/>
-    <hyperlink ref="K35" r:id="rId177" xr:uid="{6CA1EB2B-F3AB-43BC-ABE2-598B3C804B5C}"/>
-    <hyperlink ref="K37" r:id="rId178" xr:uid="{ABFE8B15-8980-4360-8CF2-634744A0EA44}"/>
-    <hyperlink ref="K38" r:id="rId179" xr:uid="{7C2539DE-C616-4420-AE0F-0F7538D09D24}"/>
-    <hyperlink ref="N40" r:id="rId180" xr:uid="{924D6220-55A2-48A1-AB46-53A3ABEF0746}"/>
-    <hyperlink ref="K40" r:id="rId181" xr:uid="{6A669A8A-5215-4AA5-848C-55DCD936C0AB}"/>
-    <hyperlink ref="K41" r:id="rId182" xr:uid="{F0DFE419-4136-4C8C-9FD8-FBC7A3BC727F}"/>
-    <hyperlink ref="K43" r:id="rId183" xr:uid="{B9DC46A9-8BFC-4EAA-B030-BA51BEDB7B9C}"/>
-    <hyperlink ref="K45" r:id="rId184" xr:uid="{4BA74EB6-9D7E-4D3D-9FAF-77E7FB196A78}"/>
-    <hyperlink ref="N46" r:id="rId185" xr:uid="{311AADDE-1447-4C6C-B031-9B62FC4CB349}"/>
-    <hyperlink ref="K46" r:id="rId186" xr:uid="{319682F7-1111-428F-B549-3D823C0473BD}"/>
-    <hyperlink ref="M44" r:id="rId187" xr:uid="{8084E5C1-6260-4BD8-9316-08B6C084562B}"/>
-    <hyperlink ref="N44" r:id="rId188" xr:uid="{3F015C13-4C64-420E-B306-F0FD87F74B03}"/>
-    <hyperlink ref="K44" r:id="rId189" xr:uid="{4E47D93A-399B-42FE-8E07-2D405816BF50}"/>
-    <hyperlink ref="K48" r:id="rId190" xr:uid="{F717B40F-09F0-4DD4-B0B6-A2F3C64E48F0}"/>
-    <hyperlink ref="K49" r:id="rId191" xr:uid="{CCF95AE5-8CD7-4306-A9B8-9BEAEF48A5FD}"/>
-    <hyperlink ref="K50" r:id="rId192" xr:uid="{99CBC954-33EE-443C-8F66-E2C938478B92}"/>
-    <hyperlink ref="K51" r:id="rId193" xr:uid="{CD3433B5-ACC2-41F5-B9BD-F469A95C3C86}"/>
-    <hyperlink ref="K52" r:id="rId194" xr:uid="{51538B87-6B8C-4F74-966A-1196020AA0E8}"/>
-    <hyperlink ref="M53" r:id="rId195" xr:uid="{7898A8F7-D259-4EA7-8C3D-0B50B4AD5BE5}"/>
-    <hyperlink ref="K53" r:id="rId196" xr:uid="{E7650F67-EF2B-4FDD-8F85-1351FFC6368B}"/>
-    <hyperlink ref="M59" r:id="rId197" xr:uid="{AFD26C96-3935-4847-A7BF-F621FCD40503}"/>
-    <hyperlink ref="N59" r:id="rId198" xr:uid="{078E6AC2-DE1D-4348-BC2C-200246F19DB2}"/>
-    <hyperlink ref="L59" r:id="rId199" xr:uid="{15EFCE8C-BEB7-40B4-9C95-70CF93574D4F}"/>
-    <hyperlink ref="K59" r:id="rId200" xr:uid="{A5A05BF8-D814-4FFF-8B5C-E156B1FAD5D1}"/>
-    <hyperlink ref="K60" r:id="rId201" xr:uid="{657AB301-10B9-4D2F-B0B2-06DF5DDD3C53}"/>
-    <hyperlink ref="K61" r:id="rId202" xr:uid="{F3B8909B-8E3C-4A6F-884A-8A987729FBBB}"/>
-    <hyperlink ref="K62" r:id="rId203" xr:uid="{27A07236-F142-4CD5-B58A-8BADFBCB20F2}"/>
-    <hyperlink ref="K63" r:id="rId204" xr:uid="{5EEF005B-21F3-49D6-B0D5-32EF60406B95}"/>
-    <hyperlink ref="K65" r:id="rId205" xr:uid="{F30C92D1-F078-4A06-865F-7ED1E78E4C37}"/>
-    <hyperlink ref="K67" r:id="rId206" xr:uid="{DC6AC5AE-9FEA-4353-A592-F01A4F3E8EFF}"/>
-    <hyperlink ref="K68" r:id="rId207" xr:uid="{52C3DC2C-29D6-485E-9652-01ECBB8E0AB4}"/>
-    <hyperlink ref="K24" r:id="rId208" xr:uid="{F4AA1EBA-46A3-4CC1-B0A3-A7B48F486807}"/>
-    <hyperlink ref="M24" r:id="rId209" xr:uid="{61A96A0E-F7E9-4F91-B970-2BACDBBDE581}"/>
-    <hyperlink ref="N24" r:id="rId210" xr:uid="{3D0A2CE0-A507-4EF1-A9ED-8A0586DB7EE2}"/>
-    <hyperlink ref="M55" r:id="rId211" xr:uid="{982BC3DA-3E52-4DB0-9FED-3F7B2BCAE0B9}"/>
-    <hyperlink ref="N55" r:id="rId212" xr:uid="{CB0562E3-426E-49BA-B17F-286E4F802A4F}"/>
-    <hyperlink ref="K55" r:id="rId213" xr:uid="{13BDE322-C3EC-4854-A29E-EB32BAF4FED7}"/>
-    <hyperlink ref="L55" r:id="rId214" xr:uid="{4D6E4DDF-06BF-4FCA-B337-BB6875D089D9}"/>
-    <hyperlink ref="K22" r:id="rId215" xr:uid="{83600694-21B2-4A2B-82C9-141CBAD64743}"/>
-    <hyperlink ref="M22" r:id="rId216" xr:uid="{D6FA8D54-F9CD-4360-8655-65CCEEB4D821}"/>
-    <hyperlink ref="N22" r:id="rId217" xr:uid="{17B2302E-1250-4C60-88EC-C0281F291EB1}"/>
-    <hyperlink ref="K23" r:id="rId218" xr:uid="{1CA12030-0275-4CFC-9B1A-785137CFB267}"/>
-    <hyperlink ref="M23" r:id="rId219" xr:uid="{3FD9CE28-B5CC-4A20-99A3-3065087AED04}"/>
-    <hyperlink ref="N23" r:id="rId220" xr:uid="{81DA205C-C4BE-43A8-A73F-A8CB6953F41E}"/>
-    <hyperlink ref="M14" r:id="rId221" xr:uid="{9809951A-64CB-4F3C-B467-66A51E760B21}"/>
-    <hyperlink ref="N50" r:id="rId222" location="!/content?menuItemDesktop=80" xr:uid="{78A67C19-4A94-41CC-83D6-9E3B0126D0C2}"/>
+    <hyperlink ref="N38" r:id="rId15" xr:uid="{36425243-7AC7-4AF2-9C5E-4565F4976C81}"/>
+    <hyperlink ref="M34" r:id="rId16" xr:uid="{DBC2D6E2-BCC2-4A50-AB7D-56020DB587FB}"/>
+    <hyperlink ref="N34" r:id="rId17" xr:uid="{2D27D948-C2E5-4F8F-B314-E0ED6384AC1F}"/>
+    <hyperlink ref="M36" r:id="rId18" xr:uid="{A07E8140-BA13-4365-A072-4B3986562265}"/>
+    <hyperlink ref="N36" r:id="rId19" xr:uid="{0971B232-3558-426C-9785-F42E3B282419}"/>
+    <hyperlink ref="M11" r:id="rId20" xr:uid="{279476CE-E1C0-48C4-818D-89FB1F97F961}"/>
+    <hyperlink ref="N11" r:id="rId21" xr:uid="{C2B01C9A-4FD2-4B15-97DE-BA135F48781E}"/>
+    <hyperlink ref="M10" r:id="rId22" xr:uid="{5B7AD2FF-5DC0-4759-B8EB-6920748A04B0}"/>
+    <hyperlink ref="N10" r:id="rId23" xr:uid="{097020E7-7110-420E-8F4F-22705FF1C983}"/>
+    <hyperlink ref="M62" r:id="rId24" xr:uid="{55DBDEEF-2AAE-4826-A696-5AF28C579F2C}"/>
+    <hyperlink ref="N62" r:id="rId25" xr:uid="{32491A74-5E35-40A2-B784-3C602FE3803E}"/>
+    <hyperlink ref="M56" r:id="rId26" xr:uid="{3326CBF8-3EB1-43A4-99CF-B30D34390DF0}"/>
+    <hyperlink ref="N56" r:id="rId27" xr:uid="{F04B0833-9438-4AA9-AD19-3E9519B662DF}"/>
+    <hyperlink ref="M26" r:id="rId28" xr:uid="{5FC295D2-0A87-43CF-B54E-E04FDEF3C086}"/>
+    <hyperlink ref="N26" r:id="rId29" xr:uid="{C69B99EC-6AAD-4348-9878-CF4948DF912F}"/>
+    <hyperlink ref="M54" r:id="rId30" xr:uid="{DA4E132F-427D-48CE-8AE5-D57D5345B0DE}"/>
+    <hyperlink ref="N54" r:id="rId31" xr:uid="{16EC9894-554A-476B-9997-8B010A26937D}"/>
+    <hyperlink ref="M28" r:id="rId32" xr:uid="{F7E5D8C3-2441-43E4-9EED-A75357EFBB21}"/>
+    <hyperlink ref="N17" r:id="rId33" xr:uid="{F05D6F16-F886-423C-ABF2-038F3B1CDEF4}"/>
+    <hyperlink ref="M17" r:id="rId34" xr:uid="{19BB88FF-CE20-4D1B-B657-42E6BD33C36F}"/>
+    <hyperlink ref="M15" r:id="rId35" xr:uid="{B0E0B30B-E083-40BC-8AA7-3338372CC3CC}"/>
+    <hyperlink ref="M13" r:id="rId36" xr:uid="{3DC141FD-85DD-4383-BEDB-EC3FFE27AAE3}"/>
+    <hyperlink ref="M12" r:id="rId37" xr:uid="{A1EEA0E6-B203-496D-BE05-7E8400174743}"/>
+    <hyperlink ref="M16" r:id="rId38" location="/overview/Wasserstand?mode=table&amp;filter=%7B%7D" xr:uid="{431514AB-B3FA-4FA0-9FAD-440C154FA405}"/>
+    <hyperlink ref="M18" r:id="rId39" xr:uid="{7D99DF82-54F7-43C9-BDF5-7393A84867EC}"/>
+    <hyperlink ref="M20" r:id="rId40" display="https://www.umwelt.sachsen.de/umwelt/infosysteme/ida/processingChain?conditionValuesSetHash=0A8BBED&amp;selector=ROOT.Thema%20Wasser.Oberirdische%20Gew%C3%A4sser.Pegel.Wasserstand%20und%20Durchfluss.OWMN%3Aowmn_menge_tagesmittelwerte_v2.sel&amp;sourceOrderAsc=false&amp;columns=9dfa2224-c924-4328-9805-1d34cd748026&amp;offset=0&amp;limit=2147483647&amp;executionConfirmed=false" xr:uid="{C35973C5-6A64-44EE-A724-C69D5BE3F7E6}"/>
+    <hyperlink ref="M21" r:id="rId41" xr:uid="{B3C90335-1BE9-48EA-B27B-E90DCED2E7E3}"/>
+    <hyperlink ref="M19" r:id="rId42" xr:uid="{39535A38-FA1B-4791-9CCF-AC09009FE4BD}"/>
+    <hyperlink ref="L20" r:id="rId43" xr:uid="{207D6C47-461A-4FB0-91AA-E9190D4AD299}"/>
+    <hyperlink ref="L14" r:id="rId44" xr:uid="{883314B1-D5D9-4628-87D5-DDE64206486E}"/>
+    <hyperlink ref="M41" r:id="rId45" xr:uid="{43926695-05CD-4BBA-8DFE-708730AA56A4}"/>
+    <hyperlink ref="M45" r:id="rId46" xr:uid="{7532A1D1-B3CC-4D73-9197-D5031B40BFAF}"/>
+    <hyperlink ref="M48" r:id="rId47" xr:uid="{47C217E4-5192-4BC5-B8DB-1689774C34DE}"/>
+    <hyperlink ref="M49" r:id="rId48" xr:uid="{0DD9DAEA-2C6C-40E8-A164-8A68BA4C893A}"/>
+    <hyperlink ref="M50" r:id="rId49" xr:uid="{D0121DD0-D1A3-4DEE-B23A-F2D5D3ABBD96}"/>
+    <hyperlink ref="M51" r:id="rId50" xr:uid="{E41A3D15-0340-41E2-98A7-F8398F4A755D}"/>
+    <hyperlink ref="N52" r:id="rId51" xr:uid="{4DAC29CC-FA65-4308-9D93-678CFFA252D6}"/>
+    <hyperlink ref="N53" r:id="rId52" xr:uid="{C40CB76B-AB6D-4BA4-8907-DED5472C6E97}"/>
+    <hyperlink ref="M3" r:id="rId53" xr:uid="{33FB1494-C397-4B17-91BC-5FE74371668D}"/>
+    <hyperlink ref="M4" r:id="rId54" xr:uid="{B8E3B2CA-F963-4B0E-8C02-4C03E1227DF4}"/>
+    <hyperlink ref="N4" r:id="rId55" xr:uid="{729A8956-37E0-4833-8991-3B8568AAFDC5}"/>
+    <hyperlink ref="M5" r:id="rId56" xr:uid="{D3531896-F25D-4B11-8143-46178B99F492}"/>
+    <hyperlink ref="M25" r:id="rId57" xr:uid="{C52B4BD9-0874-4857-AC72-F04C4D64C703}"/>
+    <hyperlink ref="M32" r:id="rId58" xr:uid="{6E3D0688-22E8-4E62-B6CA-7826AC97D1BD}"/>
+    <hyperlink ref="M33" r:id="rId59" xr:uid="{B0E296EC-DA7A-4CDB-B302-AB0BCA9A449C}"/>
+    <hyperlink ref="M37" r:id="rId60" location="Flow" xr:uid="{CDF25C43-EC31-4721-9269-ADC87A23284B}"/>
+    <hyperlink ref="M38" r:id="rId61" xr:uid="{74B57653-6E77-49EA-ACF6-F96EBEF7ABD0}"/>
+    <hyperlink ref="N37" r:id="rId62" location="Flow" xr:uid="{3A19F3BE-B518-49A6-B35C-315D0EA8F950}"/>
+    <hyperlink ref="M60" r:id="rId63" location="/publiek/waterafvoer" xr:uid="{96586330-2B0F-4F2C-8680-F6817AEB8F04}"/>
+    <hyperlink ref="M61" r:id="rId64" xr:uid="{7CC951DB-46BB-4141-91A9-CAD87A9630C2}"/>
+    <hyperlink ref="N63" r:id="rId65" xr:uid="{789C1C9F-19EE-4C2D-8BD8-94FE0B3FC6AE}"/>
+    <hyperlink ref="N68" r:id="rId66" xr:uid="{A13F99C2-CBCA-4A9C-98C1-BFCC028A369E}"/>
+    <hyperlink ref="L2" r:id="rId67" xr:uid="{0299DE14-E216-4750-86E9-8D8EB4F2F60F}"/>
+    <hyperlink ref="L4" r:id="rId68" xr:uid="{DF7D6F98-A06C-4878-8DB9-D216C854E14D}"/>
+    <hyperlink ref="L5" r:id="rId69" xr:uid="{6881C1FC-83D3-4B48-A703-2E808EF26433}"/>
+    <hyperlink ref="L6" r:id="rId70" xr:uid="{EE8683AF-647E-44D0-9AAF-DE6C59A8E670}"/>
+    <hyperlink ref="L7" r:id="rId71" xr:uid="{DA89D6B4-E546-4384-833D-5B981EB9F619}"/>
+    <hyperlink ref="L9" r:id="rId72" xr:uid="{9DBBDB5C-6C84-4AB3-A69C-456D02F16E75}"/>
+    <hyperlink ref="L11" r:id="rId73" xr:uid="{D6A5B413-7EA0-43FE-AB42-21F8D0E984F9}"/>
+    <hyperlink ref="L26" r:id="rId74" xr:uid="{FEC4CB21-36E5-4529-9BD1-0965488594A6}"/>
+    <hyperlink ref="L31" r:id="rId75" xr:uid="{F8CEB9F3-7B0C-4D96-A220-52A24EAC71E7}"/>
+    <hyperlink ref="L36" r:id="rId76" xr:uid="{EA1D39A9-DDA4-45AC-8128-015822DB9A5D}"/>
+    <hyperlink ref="L42" r:id="rId77" xr:uid="{6F22F521-9893-41B8-A862-C1942E31D4BF}"/>
+    <hyperlink ref="L54" r:id="rId78" xr:uid="{096C2498-87C2-4EF8-BA1F-5292F90C701F}"/>
+    <hyperlink ref="L56" r:id="rId79" xr:uid="{FCCB7294-9C23-47BB-B1C6-60A7018BA619}"/>
+    <hyperlink ref="L57" r:id="rId80" xr:uid="{05116FA7-B29F-4F36-AF29-282D72A106D9}"/>
+    <hyperlink ref="L58" r:id="rId81" xr:uid="{6C2CBE78-01AB-4051-8C7B-42327679A546}"/>
+    <hyperlink ref="L64" r:id="rId82" xr:uid="{923E7558-C9F5-45F4-83BD-D269E0DB6478}"/>
+    <hyperlink ref="L66" r:id="rId83" xr:uid="{F538C2FD-1BF4-46EA-9EE2-7BD3FC3454AF}"/>
+    <hyperlink ref="L69" r:id="rId84" xr:uid="{89748D0F-FE77-4F73-88FF-D48215C8E0C4}"/>
+    <hyperlink ref="L70" r:id="rId85" xr:uid="{D040ECFD-5D11-440E-903F-88818593C862}"/>
+    <hyperlink ref="L71" r:id="rId86" xr:uid="{D7BDD944-60B6-4AF0-853D-1A3F20EF5B74}"/>
+    <hyperlink ref="L8" r:id="rId87" xr:uid="{D00FA835-7423-4F1B-A2F7-7CA692EB4D08}"/>
+    <hyperlink ref="L10" r:id="rId88" xr:uid="{0950615F-A860-49D2-8DC3-F1A766019300}"/>
+    <hyperlink ref="L25" r:id="rId89" xr:uid="{6F5B7FA1-7FF8-45A0-AD6F-DAB544653875}"/>
+    <hyperlink ref="L28" r:id="rId90" xr:uid="{E23A4653-97A1-4A9C-9A5E-86DB637385CD}"/>
+    <hyperlink ref="L30" r:id="rId91" xr:uid="{B4AD2D64-E0A7-42D7-8193-9DFA2C7DC3E3}"/>
+    <hyperlink ref="L32" r:id="rId92" xr:uid="{908964D2-BFBF-4D62-8C00-9DB0F3CF8F4C}"/>
+    <hyperlink ref="L34" r:id="rId93" xr:uid="{5EAC2889-2641-4CD3-AF8D-76999ADB2175}"/>
+    <hyperlink ref="L37" r:id="rId94" location="Disclaimer" xr:uid="{3D3FE31F-229F-4DF0-B134-74A89311E685}"/>
+    <hyperlink ref="L38" r:id="rId95" location="license" xr:uid="{B99B8BD6-D4A5-453B-AE98-CC9D29CF5153}"/>
+    <hyperlink ref="L60" r:id="rId96" location="/copyright" xr:uid="{FC405A94-92ED-4C9A-B03B-2E789AC1840B}"/>
+    <hyperlink ref="L61" r:id="rId97" xr:uid="{4679CB8D-3930-4582-8DC6-6CCCD9244845}"/>
+    <hyperlink ref="L62" r:id="rId98" xr:uid="{FEB0A51B-B691-42DE-BB37-0046CEF421D3}"/>
+    <hyperlink ref="L67" r:id="rId99" xr:uid="{4052B3D9-0526-4DBE-864A-2CC2235E7A37}"/>
+    <hyperlink ref="L68" r:id="rId100" xr:uid="{CCC7D3D2-0EC0-4146-A122-99610EFB2686}"/>
+    <hyperlink ref="L15" r:id="rId101" xr:uid="{56B414F3-175F-401F-8F3A-B8C78A7999CD}"/>
+    <hyperlink ref="L13" r:id="rId102" xr:uid="{A4EAB253-FEFD-4D34-80C7-7BA329647C14}"/>
+    <hyperlink ref="L12" r:id="rId103" xr:uid="{96A4267D-73B0-4C6F-9E07-E63600BC735E}"/>
+    <hyperlink ref="L17" r:id="rId104" xr:uid="{0197946F-7B35-4321-9287-CDA7E7C977D4}"/>
+    <hyperlink ref="L18" r:id="rId105" xr:uid="{055CF3B6-9FBF-4B8C-8FD8-0AAB65FAA1E5}"/>
+    <hyperlink ref="L19" r:id="rId106" xr:uid="{3A2597C8-4F13-4689-9AFE-21B00D45BEED}"/>
+    <hyperlink ref="L21" r:id="rId107" xr:uid="{36911D06-4E86-4336-AB05-DEEFC03993C4}"/>
+    <hyperlink ref="M47" r:id="rId108" xr:uid="{EEE7B747-EA92-4E2F-8DD2-42A7E93FC151}"/>
+    <hyperlink ref="L47" r:id="rId109" xr:uid="{7CEF2492-538E-4BAD-9D26-C242373BBC4E}"/>
+    <hyperlink ref="L50" r:id="rId110" xr:uid="{DF4077F2-C770-40DD-A27F-83A17C16C2E5}"/>
+    <hyperlink ref="L48" r:id="rId111" xr:uid="{5914BA4C-2BA2-43E3-89D7-0D6B9190240E}"/>
+    <hyperlink ref="N49" r:id="rId112" xr:uid="{A817B0D0-793B-4CEB-A87B-CC6EB2B9F74F}"/>
+    <hyperlink ref="M52" r:id="rId113" xr:uid="{15DC8865-310D-4087-8466-6245886B5D29}"/>
+    <hyperlink ref="M40" r:id="rId114" xr:uid="{06D3FF73-6B12-4BBB-A197-CA12AD356B9D}"/>
+    <hyperlink ref="L35" r:id="rId115" xr:uid="{3D0FC602-9EAD-4C95-ACD5-A517F3CA367E}"/>
+    <hyperlink ref="M35" r:id="rId116" xr:uid="{5225E5E6-68CA-45D3-957A-E0E37EA3F330}"/>
+    <hyperlink ref="N35" r:id="rId117" xr:uid="{1B63C25C-317F-43E7-B1F7-5EC348C8D37F}"/>
+    <hyperlink ref="N12" r:id="rId118" xr:uid="{5191E8D6-EFCE-47F2-BFDD-65E782D29C97}"/>
+    <hyperlink ref="N13" r:id="rId119" xr:uid="{AC024018-7240-4497-9263-E5140DE193E2}"/>
+    <hyperlink ref="N14" r:id="rId120" xr:uid="{8A87FECF-B3BD-4862-B096-08E217FACC71}"/>
+    <hyperlink ref="N15" r:id="rId121" xr:uid="{B76E7E82-13F4-49FF-B9D8-936CACFEE75B}"/>
+    <hyperlink ref="N16" r:id="rId122" location="/overview/Wasserstand?mode=table&amp;filter=%7B%7D" xr:uid="{A702C0F3-C827-4E97-926E-3859C4A9F3A6}"/>
+    <hyperlink ref="N18" r:id="rId123" xr:uid="{1BDC5B18-0D62-4B9D-B3FC-EF429CD15631}"/>
+    <hyperlink ref="N19" r:id="rId124" xr:uid="{432A0A37-FCCE-437D-8B15-29AAEBAFAFEF}"/>
+    <hyperlink ref="N20" r:id="rId125" display="https://www.umwelt.sachsen.de/umwelt/infosysteme/ida/processingChain?conditionValuesSetHash=0A8BBED&amp;selector=ROOT.Thema%20Wasser.Oberirdische%20Gew%C3%A4sser.Pegel.Wasserstand%20und%20Durchfluss.OWMN%3Aowmn_menge_tagesmittelwerte_v2.sel&amp;sourceOrderAsc=false&amp;columns=9dfa2224-c924-4328-9805-1d34cd748026&amp;offset=0&amp;limit=2147483647&amp;executionConfirmed=false" xr:uid="{44371C46-89E1-42BB-8255-2F19865CAC42}"/>
+    <hyperlink ref="N21" r:id="rId126" xr:uid="{4E9346F0-3C12-486C-80E9-1D27EF91D279}"/>
+    <hyperlink ref="N28" r:id="rId127" xr:uid="{0548E784-EC86-422C-AEFF-0EB8A5B0B2D6}"/>
+    <hyperlink ref="M46" r:id="rId128" xr:uid="{EA54538E-62F8-4C22-8A62-E9926A6A5737}"/>
+    <hyperlink ref="K2" r:id="rId129" xr:uid="{39BD2D35-9444-4862-A80F-55A1E85CDBC1}"/>
+    <hyperlink ref="K3" r:id="rId130" xr:uid="{7CD1346D-FDE6-4779-937A-01DE1647C6BE}"/>
+    <hyperlink ref="K4" r:id="rId131" xr:uid="{664B96AA-17CD-4E97-8794-2B528D15B646}"/>
+    <hyperlink ref="K5" r:id="rId132" xr:uid="{95D42C21-00AD-4526-AF1D-1245D8BBDBAC}"/>
+    <hyperlink ref="K6" r:id="rId133" xr:uid="{74B0C055-27A6-4831-BF2E-BEB7443EC0BF}"/>
+    <hyperlink ref="K7" r:id="rId134" xr:uid="{53240E1F-B2EA-4CBB-BC4D-11DF789DE658}"/>
+    <hyperlink ref="K8" r:id="rId135" xr:uid="{A4D39D4C-3051-4EA7-8C35-A9F991BFE999}"/>
+    <hyperlink ref="K9" r:id="rId136" xr:uid="{7BD9B41B-78AE-4FFA-820D-B582535F5787}"/>
+    <hyperlink ref="K11" r:id="rId137" xr:uid="{A2FF850A-9C56-426B-A8D3-7699203241CA}"/>
+    <hyperlink ref="K26" r:id="rId138" xr:uid="{A9A6F852-880A-46EE-A4C6-77C5718A3201}"/>
+    <hyperlink ref="K31" r:id="rId139" xr:uid="{3E3F1C4F-BC6F-40BB-906B-FC038E31F7FA}"/>
+    <hyperlink ref="K36" r:id="rId140" xr:uid="{205D0983-3D75-4845-A2B7-F2FE9CDE7471}"/>
+    <hyperlink ref="K42" r:id="rId141" xr:uid="{5981BD4E-3A64-4044-8F00-D6CA30DFA79D}"/>
+    <hyperlink ref="K54" r:id="rId142" xr:uid="{7FB92A2C-7602-4910-82F1-6CEDDF5D9B9A}"/>
+    <hyperlink ref="K56" r:id="rId143" xr:uid="{67C930FE-1C69-449C-B47B-4A7A250402E9}"/>
+    <hyperlink ref="K57" r:id="rId144" xr:uid="{84C56357-09DE-4C90-85DB-1792BB5FD67E}"/>
+    <hyperlink ref="K58" r:id="rId145" xr:uid="{5F7107D3-8EFA-4786-84E2-A6989793C4C1}"/>
+    <hyperlink ref="K64" r:id="rId146" xr:uid="{BB77463F-FCF5-4AB6-87DD-898851A69AAF}"/>
+    <hyperlink ref="K66" r:id="rId147" xr:uid="{B0FC0A8B-D1B5-43EB-8ACC-94F2484F2473}"/>
+    <hyperlink ref="K69" r:id="rId148" xr:uid="{87F3D8E6-B39E-422F-9126-E039037C3E60}"/>
+    <hyperlink ref="K70" r:id="rId149" xr:uid="{01C03372-5C1F-4B2B-B3A5-EBDAC3883D12}"/>
+    <hyperlink ref="K71" r:id="rId150" xr:uid="{37BC70ED-F49B-4D64-A2FC-DCFD47E4FED3}"/>
+    <hyperlink ref="K10" r:id="rId151" xr:uid="{C7CF1733-E812-4526-876F-58DD8A4833F5}"/>
+    <hyperlink ref="K12" r:id="rId152" xr:uid="{A78CA3AE-B607-4503-AE9C-F1BAB092660D}"/>
+    <hyperlink ref="K13" r:id="rId153" xr:uid="{90B567F9-2099-45DB-BC2A-F72365264C51}"/>
+    <hyperlink ref="K14" r:id="rId154" xr:uid="{4DABE13E-10F9-472D-AFC4-2194D25E99D4}"/>
+    <hyperlink ref="K15" r:id="rId155" xr:uid="{63F30CC4-6855-4998-8F05-CF67C966A2C0}"/>
+    <hyperlink ref="K16" r:id="rId156" xr:uid="{18AA6A95-4D23-4770-A296-75B7DCB97DD7}"/>
+    <hyperlink ref="K17" r:id="rId157" xr:uid="{C1F270AF-7F6D-4162-80BC-558BF58E1E7C}"/>
+    <hyperlink ref="K18" r:id="rId158" xr:uid="{7E85EBA1-47D1-4E78-9C9F-CBD8CFB9A33A}"/>
+    <hyperlink ref="K19" r:id="rId159" xr:uid="{538A5124-FD86-47B8-9C9C-74CD88DACC39}"/>
+    <hyperlink ref="K20" r:id="rId160" xr:uid="{2EAE1522-545A-4EDF-8035-59C73436A4E2}"/>
+    <hyperlink ref="K21" r:id="rId161" xr:uid="{02F0BCE1-47EA-4B5C-804D-63003D4E1256}"/>
+    <hyperlink ref="K25" r:id="rId162" xr:uid="{14C3752A-1073-4D2C-A4B1-6241C66A0956}"/>
+    <hyperlink ref="K27" r:id="rId163" xr:uid="{0A765B89-5D1E-4011-A3BE-F4A4A4943B63}"/>
+    <hyperlink ref="N27" r:id="rId164" xr:uid="{9BAF5DDB-652F-4D4E-903E-C9CFA2E50E7A}"/>
+    <hyperlink ref="K28" r:id="rId165" xr:uid="{848721C6-ABF0-45B7-B5C2-EB7EFBE5073B}"/>
+    <hyperlink ref="K29" r:id="rId166" xr:uid="{E36B8C29-A364-4F36-8A5A-52E09808BEED}"/>
+    <hyperlink ref="K30" r:id="rId167" xr:uid="{E8ED1CD5-2249-4B8B-9940-6E1A699441C1}"/>
+    <hyperlink ref="K32" r:id="rId168" xr:uid="{F057875F-AA86-468C-97C4-935E7ADDCDF1}"/>
+    <hyperlink ref="K33" r:id="rId169" xr:uid="{FDD7E05C-4786-4A71-B881-CEC77A8E45BE}"/>
+    <hyperlink ref="K34" r:id="rId170" xr:uid="{96BD0EB1-795E-42C6-BBB6-EF0E987EAD0F}"/>
+    <hyperlink ref="K35" r:id="rId171" xr:uid="{6CA1EB2B-F3AB-43BC-ABE2-598B3C804B5C}"/>
+    <hyperlink ref="K37" r:id="rId172" xr:uid="{ABFE8B15-8980-4360-8CF2-634744A0EA44}"/>
+    <hyperlink ref="K38" r:id="rId173" xr:uid="{7C2539DE-C616-4420-AE0F-0F7538D09D24}"/>
+    <hyperlink ref="N40" r:id="rId174" xr:uid="{924D6220-55A2-48A1-AB46-53A3ABEF0746}"/>
+    <hyperlink ref="K40" r:id="rId175" xr:uid="{6A669A8A-5215-4AA5-848C-55DCD936C0AB}"/>
+    <hyperlink ref="K41" r:id="rId176" xr:uid="{F0DFE419-4136-4C8C-9FD8-FBC7A3BC727F}"/>
+    <hyperlink ref="K43" r:id="rId177" xr:uid="{B9DC46A9-8BFC-4EAA-B030-BA51BEDB7B9C}"/>
+    <hyperlink ref="K45" r:id="rId178" xr:uid="{4BA74EB6-9D7E-4D3D-9FAF-77E7FB196A78}"/>
+    <hyperlink ref="N46" r:id="rId179" xr:uid="{311AADDE-1447-4C6C-B031-9B62FC4CB349}"/>
+    <hyperlink ref="K46" r:id="rId180" xr:uid="{319682F7-1111-428F-B549-3D823C0473BD}"/>
+    <hyperlink ref="M44" r:id="rId181" xr:uid="{8084E5C1-6260-4BD8-9316-08B6C084562B}"/>
+    <hyperlink ref="N44" r:id="rId182" xr:uid="{3F015C13-4C64-420E-B306-F0FD87F74B03}"/>
+    <hyperlink ref="K44" r:id="rId183" xr:uid="{4E47D93A-399B-42FE-8E07-2D405816BF50}"/>
+    <hyperlink ref="K48" r:id="rId184" xr:uid="{F717B40F-09F0-4DD4-B0B6-A2F3C64E48F0}"/>
+    <hyperlink ref="K49" r:id="rId185" xr:uid="{CCF95AE5-8CD7-4306-A9B8-9BEAEF48A5FD}"/>
+    <hyperlink ref="K50" r:id="rId186" xr:uid="{99CBC954-33EE-443C-8F66-E2C938478B92}"/>
+    <hyperlink ref="K51" r:id="rId187" xr:uid="{CD3433B5-ACC2-41F5-B9BD-F469A95C3C86}"/>
+    <hyperlink ref="K52" r:id="rId188" xr:uid="{51538B87-6B8C-4F74-966A-1196020AA0E8}"/>
+    <hyperlink ref="M53" r:id="rId189" xr:uid="{7898A8F7-D259-4EA7-8C3D-0B50B4AD5BE5}"/>
+    <hyperlink ref="K53" r:id="rId190" xr:uid="{E7650F67-EF2B-4FDD-8F85-1351FFC6368B}"/>
+    <hyperlink ref="M59" r:id="rId191" xr:uid="{AFD26C96-3935-4847-A7BF-F621FCD40503}"/>
+    <hyperlink ref="N59" r:id="rId192" xr:uid="{078E6AC2-DE1D-4348-BC2C-200246F19DB2}"/>
+    <hyperlink ref="L59" r:id="rId193" xr:uid="{15EFCE8C-BEB7-40B4-9C95-70CF93574D4F}"/>
+    <hyperlink ref="K59" r:id="rId194" xr:uid="{A5A05BF8-D814-4FFF-8B5C-E156B1FAD5D1}"/>
+    <hyperlink ref="K60" r:id="rId195" xr:uid="{657AB301-10B9-4D2F-B0B2-06DF5DDD3C53}"/>
+    <hyperlink ref="K61" r:id="rId196" xr:uid="{F3B8909B-8E3C-4A6F-884A-8A987729FBBB}"/>
+    <hyperlink ref="K62" r:id="rId197" xr:uid="{27A07236-F142-4CD5-B58A-8BADFBCB20F2}"/>
+    <hyperlink ref="K63" r:id="rId198" xr:uid="{5EEF005B-21F3-49D6-B0D5-32EF60406B95}"/>
+    <hyperlink ref="K67" r:id="rId199" xr:uid="{DC6AC5AE-9FEA-4353-A592-F01A4F3E8EFF}"/>
+    <hyperlink ref="K68" r:id="rId200" xr:uid="{52C3DC2C-29D6-485E-9652-01ECBB8E0AB4}"/>
+    <hyperlink ref="K24" r:id="rId201" xr:uid="{F4AA1EBA-46A3-4CC1-B0A3-A7B48F486807}"/>
+    <hyperlink ref="M24" r:id="rId202" xr:uid="{61A96A0E-F7E9-4F91-B970-2BACDBBDE581}"/>
+    <hyperlink ref="N24" r:id="rId203" xr:uid="{3D0A2CE0-A507-4EF1-A9ED-8A0586DB7EE2}"/>
+    <hyperlink ref="M55" r:id="rId204" xr:uid="{982BC3DA-3E52-4DB0-9FED-3F7B2BCAE0B9}"/>
+    <hyperlink ref="N55" r:id="rId205" xr:uid="{CB0562E3-426E-49BA-B17F-286E4F802A4F}"/>
+    <hyperlink ref="K55" r:id="rId206" xr:uid="{13BDE322-C3EC-4854-A29E-EB32BAF4FED7}"/>
+    <hyperlink ref="L55" r:id="rId207" xr:uid="{4D6E4DDF-06BF-4FCA-B337-BB6875D089D9}"/>
+    <hyperlink ref="K22" r:id="rId208" xr:uid="{83600694-21B2-4A2B-82C9-141CBAD64743}"/>
+    <hyperlink ref="M22" r:id="rId209" xr:uid="{D6FA8D54-F9CD-4360-8655-65CCEEB4D821}"/>
+    <hyperlink ref="N22" r:id="rId210" xr:uid="{17B2302E-1250-4C60-88EC-C0281F291EB1}"/>
+    <hyperlink ref="K23" r:id="rId211" xr:uid="{1CA12030-0275-4CFC-9B1A-785137CFB267}"/>
+    <hyperlink ref="M23" r:id="rId212" xr:uid="{3FD9CE28-B5CC-4A20-99A3-3065087AED04}"/>
+    <hyperlink ref="N23" r:id="rId213" xr:uid="{81DA205C-C4BE-43A8-A73F-A8CB6953F41E}"/>
+    <hyperlink ref="M14" r:id="rId214" xr:uid="{9809951A-64CB-4F3C-B467-66A51E760B21}"/>
+    <hyperlink ref="N50" r:id="rId215" location="!/content?menuItemDesktop=80" xr:uid="{78A67C19-4A94-41CC-83D6-9E3B0126D0C2}"/>
+    <hyperlink ref="L65" r:id="rId216" xr:uid="{AD51A4A5-D5FA-4E5C-8D92-BFFDD78E9CCD}"/>
+    <hyperlink ref="K65" r:id="rId217" xr:uid="{A0792139-9A4B-4ED3-AACA-645856CB775F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5278,72 +5272,72 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Some main adjusts, but mainly new names (area)
</commit_message>
<xml_diff>
--- a/data/streamflow/estreams_streamflow_catalogue.xlsx
+++ b/data/streamflow/estreams_streamflow_catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b65690e0ed38c20/PhD/Eawag/Papers/Paper1_Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b65690e0ed38c20/PhD/Eawag/Papers/Paper1_Database/Paper/data/streamflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C14E6D5-EA83-4050-B4A2-F22553A8D8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{D6F04766-2B18-4166-A0A0-6A19CFC91086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CF2DAF6-BDC8-334E-9577-DC09AC50D13F}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{440C78F0-496D-5848-B483-D1372D576F79}"/>
+    <workbookView xWindow="29400" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{440C78F0-496D-5848-B483-D1372D576F79}"/>
   </bookViews>
   <sheets>
     <sheet name="catalogue" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="476">
   <si>
     <t>provider_id</t>
   </si>
@@ -87,6 +87,9 @@
     <t>observations</t>
   </si>
   <si>
+    <t>download_method</t>
+  </si>
+  <si>
     <t>AT_EHYD</t>
   </si>
   <si>
@@ -120,10 +123,7 @@
     <t>BA</t>
   </si>
   <si>
-    <t>Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t>BO</t>
+    <t>BOSNIA AND HERZEGOVINA</t>
   </si>
   <si>
     <t>Federalni hidrometeorološki zavod (FHMZ)</t>
@@ -251,6 +251,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Höge, M. </t>
     </r>
@@ -260,6 +261,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>et al.</t>
     </r>
@@ -268,6 +270,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t> CAMELS-CH: hydro-meteorological time series and landscape attributes for 331 catchments in hydrologic Switzerland. </t>
     </r>
@@ -277,6 +280,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Earth Syst Sci Data</t>
     </r>
@@ -285,6 +289,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -294,6 +299,7 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>15</t>
     </r>
@@ -302,8 +308,9 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
-      <t>, 5755–5784 (2023); BAFU. Federal Office for the Environment, Switzerland. https://www.bafu.admin.ch/bafu/en/home.html (last access: 15 May 2023).</t>
+      <t>, 5755–5784 (2023); BAFU. Federal Office for the Environment, Switzerland. https://www.bafu.admin.ch/bafu/en/home.html (last access: 15 May 2023); BAFU. Federal Office for the Environment, Switzerland. https://www.bafu.admin.ch/bafu/en/home.html (last access: 15 May 2023).</t>
     </r>
   </si>
   <si>
@@ -331,13 +338,10 @@
     <t>Český hydrometeorologický ústav (CHMU)</t>
   </si>
   <si>
-    <t>CC BY-NC-ND 3.0</t>
-  </si>
-  <si>
     <t>https://isvs.chmi.cz</t>
   </si>
   <si>
-    <t>https://www.chmi.cz/podminky-uziti; https://creativecommons.org/licenses/by-nc-nd/3.0/cz/</t>
+    <t>https://isvs.chmi.cz/ords/chmi_app/r/11002/files/static/v5/chmu/podmCHMU.pdf</t>
   </si>
   <si>
     <t>https://isvs.chmi.cz/ords/f?p=11002:HOME:5026647009329:::::</t>
@@ -424,9 +428,6 @@
     <t>Bayerisches Landesamt fur Umwelt (GKD Bayern)</t>
   </si>
   <si>
-    <t>Redristribution allowed</t>
-  </si>
-  <si>
     <t>https://www.gkd.bayern.de/en/</t>
   </si>
   <si>
@@ -490,6 +491,9 @@
     <t>ELWAS-WEB. Ministerium fur Umwelt, Naturschutz und Verkehr des Landes Nordrhein-Westfalen, https://www.elwasweb.nrw.de/elwas-web/data-objekt;jsessionid=DADDD7196B89E206917D18793294E375;jsessionid=F76CC7CC8ECFBA5F518ECD241AF0BA78?art=Pegel (last access: 12 Dec 2023).</t>
   </si>
   <si>
+    <t>To download all stations at once: 1. Check the panel “Oberflachengwasser”, and choose “Pegel” under “Menge”; 2. Then make sure your variable (“Hauptwerte”) is set to average discharge “MQ –Mittlerer Abfluss”. The you can just click “Suchen” search, and all stations will be visible; 3. Then tick the box at the top to select all stations; 4. Now you can download an excel with the metadata of all stations by choosing “Excel Export”. To download the timeseries click “Export Abflussdaten”.</t>
+  </si>
+  <si>
     <t>DE_SH</t>
   </si>
   <si>
@@ -619,7 +623,7 @@
     <t>ODA. Overfladevandsdatabasen: Aarhus University, Denmark. https://odaforalle.au.dk/login.aspx (last access: 17 Jul 2023).</t>
   </si>
   <si>
-    <t xml:space="preserve">One needs to leave their e-mail to access the data. </t>
+    <t xml:space="preserve"># For the streamflow records: 1. First you need to leave your e-mail address; 2. Click on “hent data”, which means get data. In the drop-down menu choose “Vandlob”. 3. Choose “Hydrometri” and then “dognvandforing” which means daily discharge. Then “ar” means year, and then you can choose an individual year or click on “valg alle” to choose every year. 4. To choose which station go to the tab of “observationsstednr” meaning observation location number. You can choose individual stations or the “valg alle”. #For catchment areas: 1. First you need to leave your e-mail address; 2. Click on "hent data" and choose ”Vandløb”; 3. Click on ”Oplandsbeskrivelse” and choose ”Oplandsareal” and then you can choose the stations in the long list and now you should get a file containing catchments areas. </t>
   </si>
   <si>
     <t>EE_GRDC</t>
@@ -688,7 +692,7 @@
     <t>FEI. Finish Environmental Institute, Finland. https://wwwp2.ymparisto.fi/scripts/kirjaudu.asp (last access: 10 Jul 2023).</t>
   </si>
   <si>
-    <t>Link to make an account: https://www.syke.fi/fi-FI/Avoin_tieto/Ymparistotietojarjestelmat/Rekisteroityminen;</t>
+    <t xml:space="preserve">1. First make an account using the link: https://www.syke.fi/fi-FI/Avoin_tieto/Ymparistotietojarjestelmat/Rekisteroityminen; 2. Once logged in: click on the "Ympäristötiedon hallintajärjestelmä Hertta" to get to the database; 3. Translate to English by first clicking on "Asetukset" and clickon “Kieli” and choose “ Englanti” for English. “Suomi” means finish. Click ok “Hyvasky” and close the pop-up ‘Sulje”. ;  4. Then you click “Hydrology &gt; Hydrological observations &gt; Data search” ; 5. The site has a maximum amount of data you can download in one go. So you need to choose an area and then search up all the stations in that area, download and then move on to the next area. One tip is to choose "county" in the tab "Area"; 6. Now you should seelct the discharge. Click on "Observation station", select "Parameter", then "Virtaama", then click on "Accept"; 7. After selecting the "Area" and the "Observation station", click on "Places on list" on the right side of the screen. You will be redirected to another page; 8. Now select the desired stations (there is a maximum) and click on "select action" &gt; "resultlist", and then select the desired time-period; 9. Now click on "to file", select the desired file format (EXCEL), then click ion "to file" again. Now you will be able to download the data; 10. Repeat until you are done with all the desired stations. </t>
   </si>
   <si>
     <t>FR_EAUFRANCE</t>
@@ -706,7 +710,7 @@
     <t>https://www.hydro.eaufrance.fr</t>
   </si>
   <si>
-    <t>BanqueHydro. Hydro Portail, France. https://www.hydro.eaufrance.fr/ (last access: 06 Jul 2023).</t>
+    <t>BanqueHydro. Hydro Portail, France. https://www.hydro.eaufrance.fr/ (last access: 01 May 2024).</t>
   </si>
   <si>
     <t>GB_NRFA</t>
@@ -1297,6 +1301,9 @@
     <t>NVE. Norwegian Water Resources and Energy Directorate, Norway. https://seriekart.nve.no (last access: 10 Jul 2023).</t>
   </si>
   <si>
+    <t xml:space="preserve">The user can either use the provided website for download the data individually, or the official API (https://hydapi.nve.no/UserDocumentation/) to download data from many stations at once. </t>
+  </si>
+  <si>
     <t>PL_IMGW</t>
   </si>
   <si>
@@ -1330,7 +1337,7 @@
     <t>PORTUGAL</t>
   </si>
   <si>
-    <t>Sistema nacional de Informacao de Recursos Hidricos (SNIRH)</t>
+    <t>Sistema Nacional de Informacao de Recursos Hidricos (SNIRH)</t>
   </si>
   <si>
     <t>https://snirh.apambiente.pt</t>
@@ -1508,13 +1515,28 @@
   </si>
   <si>
     <t>attributes_aggreation_landscape_landcover.js</t>
+  </si>
+  <si>
+    <t>Downloadable all at once</t>
+  </si>
+  <si>
+    <t>Code provided by EStreams</t>
+  </si>
+  <si>
+    <t>Downloadable individually</t>
+  </si>
+  <si>
+    <t>Download via request form</t>
+  </si>
+  <si>
+    <t>API by the official provider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1540,12 +1562,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1553,12 +1577,14 @@
       <sz val="9"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1593,18 +1619,29 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1641,7 +1678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1651,7 +1688,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1666,11 +1702,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1687,9 +1722,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1727,7 +1762,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1833,7 +1868,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1975,7 +2010,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1983,35 +2018,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71BA99F6-C102-264A-9C07-16ADE26DD985}">
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C23" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E40" sqref="E40"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.375" customWidth="1"/>
-    <col min="10" max="10" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" style="10" customWidth="1"/>
-    <col min="12" max="12" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="13.625" customWidth="1"/>
-    <col min="15" max="15" width="187.125" customWidth="1"/>
-    <col min="16" max="16" width="191.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="187.1640625" customWidth="1"/>
+    <col min="16" max="16" width="191.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -2059,70 +2095,77 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="O2" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="R2" s="15"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -2131,7 +2174,7 @@
         <v>30</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>31</v>
@@ -2139,12 +2182,15 @@
       <c r="N3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>33</v>
       </c>
@@ -2164,7 +2210,7 @@
         <v>38</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -2181,12 +2227,15 @@
       <c r="N4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="11" t="s">
         <v>42</v>
       </c>
       <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>43</v>
       </c>
@@ -2206,7 +2255,7 @@
         <v>46</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -2223,12 +2272,15 @@
       <c r="N5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="11" t="s">
         <v>50</v>
       </c>
       <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>51</v>
       </c>
@@ -2248,7 +2300,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2265,12 +2317,15 @@
       <c r="N6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>59</v>
       </c>
@@ -2290,7 +2345,7 @@
         <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2307,12 +2362,15 @@
       <c r="N7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>63</v>
       </c>
@@ -2332,7 +2390,7 @@
         <v>67</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2349,12 +2407,15 @@
       <c r="N8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>69</v>
       </c>
       <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>70</v>
       </c>
@@ -2374,7 +2435,7 @@
         <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2391,12 +2452,15 @@
       <c r="N9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>74</v>
       </c>
@@ -2413,37 +2477,40 @@
         <v>77</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="N10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="O10" s="12" t="s">
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>76</v>
@@ -2458,7 +2525,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2475,626 +2542,673 @@
       <c r="N11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="O11" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="4" t="str">
+        <f t="shared" ref="B12:B21" si="0">_xlfn.CONCAT(LEFT(A12,2), RIGHT(A12,2))</f>
+        <v>DEBB</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A12,2), RIGHT(A12,2))</f>
-        <v>DEBB</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="G12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="N12" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="6" t="s">
+      <c r="B13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DEBE</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A13,2), RIGHT(A13,2))</f>
-        <v>DEBE</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="N13" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="O13" s="12" t="s">
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DEBW</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A14,2), RIGHT(A14,2))</f>
-        <v>DEBW</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="N14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="O14" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="N14" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="O14" s="12" t="s">
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DEBY</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A15,2), RIGHT(A15,2))</f>
-        <v>DEBY</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="N15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O15" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="N15" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="O15" s="12" t="s">
+      <c r="B16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DEHE</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A16,2), RIGHT(A16,2))</f>
-        <v>DEHE</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="O16" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="5" t="s">
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="N16" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="O16" s="12" t="s">
+      <c r="B17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DENI</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A17,2), RIGHT(A17,2))</f>
-        <v>DENI</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="N17" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="O17" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="N17" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O17" s="12" t="s">
+      <c r="B18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DENW</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A18,2), RIGHT(A18,2))</f>
-        <v>DENW</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="N18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O18" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="P18" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="N18" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="O18" s="14" t="s">
+      <c r="Q18" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DESH</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A19,2), RIGHT(A19,2))</f>
-        <v>DESH</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>133</v>
-      </c>
       <c r="G19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="N19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="O19" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="N19" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="O19" s="14" t="s">
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DESN</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A20,2), RIGHT(A20,2))</f>
-        <v>DESN</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="N20" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="N20" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="O20" s="14" t="s">
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>DEST</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="4" t="str">
-        <f>_xlfn.CONCAT(LEFT(A21,2), RIGHT(A21,2))</f>
-        <v>DEST</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="M21" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="O21" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="N21" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="O21" s="12" t="s">
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="4" t="str">
+        <f t="shared" ref="B22:B24" si="1">_xlfn.CONCAT(LEFT(A22,2), RIGHT(A22,2))</f>
+        <v>DETH</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="4" t="str">
-        <f t="shared" ref="B22:B24" si="0">_xlfn.CONCAT(LEFT(A22,2), RIGHT(A22,2))</f>
-        <v>DETH</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="L22" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="15" t="s">
+      <c r="N22" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="O22" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="N22" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="O22" s="12" t="s">
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DEBU</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>DEBU</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="15" t="s">
+      <c r="N23" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="O23" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N23" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="O23" s="12" t="s">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DERP</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>DERP</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>161</v>
-      </c>
       <c r="F24" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="15" t="s">
+      <c r="K24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L24" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="M24" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="M24" s="5" t="s">
+      <c r="N24" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="O24" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="N24" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="O24" s="12" t="s">
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>170</v>
-      </c>
       <c r="G25" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="O25" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="M25" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="O25" s="12" t="s">
+      <c r="P25" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="P25" s="4" t="s">
+      <c r="Q25" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>55</v>
@@ -3103,7 +3217,7 @@
         <v>38</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -3120,197 +3234,212 @@
       <c r="N26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O26" s="12" t="s">
+      <c r="O26" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P26" s="4"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>182</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="L27" s="7" t="s">
+      <c r="M27" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="N27" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="O27" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="N27" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="O27" s="12" t="s">
+      <c r="P27" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="P27" s="4" t="s">
+      <c r="Q27" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="G28" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="L28" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="N28" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O28" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="N28" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="O28" s="12" t="s">
+      <c r="P28" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="P28" s="4" t="s">
+      <c r="Q28" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>201</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="O29" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M29" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="N29" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="O29" s="12" t="s">
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="N30" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="O30" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="N30" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="O30" s="12" t="s">
+      <c r="P30" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="P30" s="4" t="s">
+      <c r="Q30" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>55</v>
@@ -3319,7 +3448,7 @@
         <v>38</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -3336,191 +3465,206 @@
       <c r="N31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O31" s="12" t="s">
+      <c r="O31" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>219</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="N32" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="O32" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="N32" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="O32" s="12" t="s">
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>226</v>
-      </c>
       <c r="F33" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="O33" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="N33" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="O33" s="12" t="s">
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="O34" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="O34" s="12" t="s">
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="1:16">
-      <c r="A35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>240</v>
-      </c>
       <c r="G35" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="M35" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="O35" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="M35" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="O35" s="12" t="s">
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>245</v>
-      </c>
       <c r="C36" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>55</v>
@@ -3529,7 +3673,7 @@
         <v>38</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -3546,233 +3690,251 @@
       <c r="N36" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O36" s="12" t="s">
+      <c r="O36" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P36" s="4"/>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="M37" s="5" t="s">
+      <c r="N37" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="O37" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="N37" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="O37" s="12" t="s">
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="P37" s="4"/>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>257</v>
-      </c>
       <c r="F38" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="L38" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="M38" s="5" t="s">
+      <c r="N38" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="O38" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="N38" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="O38" s="12" t="s">
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="P38" s="4"/>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="A39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>265</v>
-      </c>
       <c r="F39" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="O39" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="L39" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="O39" s="12" t="s">
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="P39" s="4"/>
-    </row>
-    <row r="40" spans="1:16">
-      <c r="A40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="L40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M40" s="5" t="s">
+      <c r="N40" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="O40" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="N40" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="O40" s="12" t="s">
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="P40" s="4"/>
-    </row>
-    <row r="41" spans="1:16">
-      <c r="A41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>278</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="N41" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="L41" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="N41" s="5" t="s">
+      <c r="O41" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="O41" s="12" t="s">
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="P41" s="4"/>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>283</v>
-      </c>
       <c r="C42" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>270</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>271</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>55</v>
@@ -3781,7 +3943,7 @@
         <v>38</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -3798,487 +3960,523 @@
       <c r="N42" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O42" s="12" t="s">
+      <c r="O42" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P42" s="4"/>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="F43" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="L43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M43" s="5" t="s">
+      <c r="N43" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="O43" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="N43" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="O43" s="12" t="s">
+      <c r="P43" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="P43" s="4" t="s">
+      <c r="Q43" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
-      <c r="A44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>293</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="L44" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M44" s="5" t="s">
+      <c r="N44" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="O44" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="N44" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="O44" s="12" t="s">
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="P44" s="4"/>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="6" t="s">
+      <c r="B45" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="C45" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>299</v>
-      </c>
       <c r="F45" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="N45" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="L45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="N45" s="5" t="s">
+      <c r="O45" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="O45" s="12" t="s">
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="P45" s="4"/>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46" s="6" t="s">
+      <c r="B46" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="L46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M46" s="5" t="s">
+      <c r="N46" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="O46" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="N46" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="O46" s="12" t="s">
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="P46" s="4"/>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="A47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="C47" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>311</v>
-      </c>
       <c r="F47" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="L47" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="L47" s="5" t="s">
+      <c r="M47" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="M47" s="5" t="s">
+      <c r="N47" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="N47" s="5" t="s">
+      <c r="O47" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="O47" s="12" t="s">
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="P47" s="4"/>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" s="6" t="s">
+      <c r="B48" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>319</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
       <c r="K48" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="L48" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="L48" s="5" t="s">
+      <c r="M48" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="N48" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="O48" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="N48" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="O48" s="12" t="s">
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="P48" s="4"/>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="A49" s="6" t="s">
+      <c r="B49" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>326</v>
-      </c>
       <c r="F49" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M49" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="L49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M49" s="5" t="s">
+      <c r="N49" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="N49" s="5" t="s">
+      <c r="O49" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="O49" s="12" t="s">
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="P49" s="4"/>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" s="6" t="s">
+      <c r="B50" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>333</v>
-      </c>
       <c r="F50" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="L50" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="L50" s="5" t="s">
+      <c r="M50" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="N50" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="M50" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="N50" s="16" t="s">
+      <c r="O50" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="O50" s="12" t="s">
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="P50" s="4"/>
-    </row>
-    <row r="51" spans="1:16">
-      <c r="A51" s="6" t="s">
+      <c r="B51" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>340</v>
-      </c>
       <c r="F51" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="N51" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="L51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="N51" s="5" t="s">
+      <c r="O51" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="O51" s="12" t="s">
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="P51" s="4"/>
-    </row>
-    <row r="52" spans="1:16">
-      <c r="A52" s="6" t="s">
+      <c r="B52" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>346</v>
-      </c>
       <c r="F52" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="O52" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="L52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="N52" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="O52" s="12" t="s">
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="P52" s="4"/>
-    </row>
-    <row r="53" spans="1:16">
-      <c r="A53" s="6" t="s">
+      <c r="B53" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="N53" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="N53" s="5" t="s">
+      <c r="O53" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="O53" s="12" t="s">
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="P53" s="4"/>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="A54" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>358</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>55</v>
@@ -4287,7 +4485,7 @@
         <v>38</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -4304,65 +4502,71 @@
       <c r="N54" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O54" s="12" t="s">
+      <c r="O54" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P54" s="4"/>
-    </row>
-    <row r="55" spans="1:16">
+      <c r="Q54" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="D55" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>362</v>
-      </c>
       <c r="F55" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="L55" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="L55" s="5" t="s">
+      <c r="M55" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="M55" s="5" t="s">
+      <c r="N55" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="O55" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="N55" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="O55" s="4" t="s">
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="P55" s="4"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>370</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>55</v>
@@ -4371,7 +4575,7 @@
         <v>38</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -4388,23 +4592,26 @@
       <c r="N56" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O56" s="12" t="s">
+      <c r="O56" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P56" s="4"/>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="Q56" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>373</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>374</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>55</v>
@@ -4413,7 +4620,7 @@
         <v>38</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -4430,23 +4637,26 @@
       <c r="N57" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O57" s="12" t="s">
+      <c r="O57" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P57" s="4"/>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>377</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>378</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>55</v>
@@ -4455,7 +4665,7 @@
         <v>38</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -4472,140 +4682,154 @@
       <c r="N58" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O58" s="12" t="s">
+      <c r="O58" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P58" s="4"/>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>381</v>
-      </c>
       <c r="D59" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L59" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="L59" s="5" t="s">
+      <c r="M59" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M59" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="N59" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="O59" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="O59" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="P59" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q59" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="P59" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16">
-      <c r="A60" s="6" t="s">
+      <c r="B60" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="D60" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="E60" s="4" t="s">
+      <c r="F60" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>387</v>
-      </c>
       <c r="G60" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="L60" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="L60" s="5" t="s">
+      <c r="M60" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="M60" s="5" t="s">
+      <c r="N60" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="O60" s="11" t="s">
         <v>390</v>
       </c>
-      <c r="N60" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="O60" s="12" t="s">
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="P60" s="4"/>
-    </row>
-    <row r="61" spans="1:16">
-      <c r="A61" s="6" t="s">
+      <c r="B61" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="D61" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="E61" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>396</v>
-      </c>
       <c r="G61" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="L61" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="L61" s="5" t="s">
+      <c r="M61" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="N61" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="O61" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="M61" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="N61" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="O61" s="12" t="s">
+      <c r="P61" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="P61" s="4"/>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="Q61" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>400</v>
       </c>
@@ -4622,10 +4846,10 @@
         <v>403</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -4636,18 +4860,21 @@
       <c r="L62" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="M62" s="5" t="s">
+      <c r="M62" s="14" t="s">
         <v>406</v>
       </c>
       <c r="N62" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="O62" s="12" t="s">
+      <c r="O62" s="11" t="s">
         <v>407</v>
       </c>
       <c r="P62" s="4"/>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>408</v>
       </c>
@@ -4664,19 +4891,19 @@
         <v>411</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
-      <c r="K63" s="15" t="s">
+      <c r="K63" s="5" t="s">
         <v>412</v>
       </c>
       <c r="L63" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M63" s="5" t="s">
         <v>413</v>
@@ -4684,14 +4911,17 @@
       <c r="N63" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="O63" s="12" t="s">
+      <c r="O63" s="11" t="s">
         <v>414</v>
       </c>
       <c r="P63" s="4" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>416</v>
       </c>
@@ -4711,7 +4941,7 @@
         <v>38</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -4728,12 +4958,15 @@
       <c r="N64" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O64" s="12" t="s">
+      <c r="O64" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P64" s="4"/>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="Q64" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>420</v>
       </c>
@@ -4753,7 +4986,7 @@
         <v>38</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
@@ -4770,12 +5003,15 @@
       <c r="N65" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O65" s="12" t="s">
+      <c r="O65" s="11" t="s">
         <v>424</v>
       </c>
       <c r="P65" s="4"/>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>425</v>
       </c>
@@ -4795,7 +5031,7 @@
         <v>38</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -4812,12 +5048,15 @@
       <c r="N66" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="12" t="s">
+      <c r="O66" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P66" s="4"/>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="Q66" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>429</v>
       </c>
@@ -4834,10 +5073,10 @@
         <v>432</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
@@ -4854,12 +5093,15 @@
       <c r="N67" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="O67" s="12" t="s">
+      <c r="O67" s="11" t="s">
         <v>436</v>
       </c>
       <c r="P67" s="4"/>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="Q67" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>437</v>
       </c>
@@ -4876,10 +5118,10 @@
         <v>440</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
@@ -4896,12 +5138,15 @@
       <c r="N68" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="O68" s="12" t="s">
+      <c r="O68" s="11" t="s">
         <v>444</v>
       </c>
       <c r="P68" s="4"/>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>445</v>
       </c>
@@ -4921,7 +5166,7 @@
         <v>38</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
@@ -4938,12 +5183,15 @@
       <c r="N69" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O69" s="12" t="s">
+      <c r="O69" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P69" s="4"/>
-    </row>
-    <row r="70" spans="1:16">
+      <c r="Q69" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>449</v>
       </c>
@@ -4963,7 +5211,7 @@
         <v>38</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -4980,12 +5228,15 @@
       <c r="N70" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O70" s="12" t="s">
+      <c r="O70" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P70" s="4"/>
-    </row>
-    <row r="71" spans="1:16">
+      <c r="Q70" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>453</v>
       </c>
@@ -5005,7 +5256,7 @@
         <v>38</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -5022,10 +5273,13 @@
       <c r="N71" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O71" s="12" t="s">
+      <c r="O71" s="11" t="s">
         <v>58</v>
       </c>
       <c r="P71" s="4"/>
+      <c r="Q71" s="4" t="s">
+        <v>471</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P71">
@@ -5262,80 +5516,80 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>470</v>
       </c>

</xml_diff>